<commit_message>
i think the dashboard is now working
</commit_message>
<xml_diff>
--- a/src/wales.xlsx
+++ b/src/wales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="309">
   <si>
     <t>customer_email</t>
   </si>
@@ -319,9 +319,6 @@
     <t>Sian Simons</t>
   </si>
   <si>
-    <t>Simon Davies</t>
-  </si>
-  <si>
     <t>Sophia Churchill</t>
   </si>
   <si>
@@ -634,9 +631,6 @@
     <t>siansimons@hotmail.co.uk</t>
   </si>
   <si>
-    <t>bigsimon@hotmail.co.uk</t>
-  </si>
-  <si>
     <t>sophiachurchill@hotmail.com</t>
   </si>
   <si>
@@ -865,82 +859,88 @@
     <t>Dec 7, 2023</t>
   </si>
   <si>
-    <t>Mar 30, 2024</t>
-  </si>
-  <si>
     <t>Mar 26, 2024</t>
   </si>
   <si>
     <t>Dec 29, 2023</t>
   </si>
   <si>
+    <t>Sep 2, 2024</t>
+  </si>
+  <si>
+    <t>Aug 29, 2024</t>
+  </si>
+  <si>
+    <t>Aug 21, 2024</t>
+  </si>
+  <si>
+    <t>Sep 1, 2024</t>
+  </si>
+  <si>
+    <t>Aug 6, 2024</t>
+  </si>
+  <si>
+    <t>Aug 17, 2024</t>
+  </si>
+  <si>
+    <t>Aug 5, 2024</t>
+  </si>
+  <si>
+    <t>Aug 27, 2024</t>
+  </si>
+  <si>
+    <t>Aug 28, 2024</t>
+  </si>
+  <si>
+    <t>Aug 3, 2024</t>
+  </si>
+  <si>
+    <t>Aug 30, 2024</t>
+  </si>
+  <si>
+    <t>Aug 13, 2024</t>
+  </si>
+  <si>
+    <t>Aug 16, 2024</t>
+  </si>
+  <si>
+    <t>Aug 12, 2024</t>
+  </si>
+  <si>
+    <t>Aug 20, 2024</t>
+  </si>
+  <si>
+    <t>Aug 4, 2024</t>
+  </si>
+  <si>
+    <t>Aug 8, 2024</t>
+  </si>
+  <si>
+    <t>Aug 11, 2024</t>
+  </si>
+  <si>
+    <t>Aug 14, 2024</t>
+  </si>
+  <si>
+    <t>Aug 18, 2024</t>
+  </si>
+  <si>
+    <t>Aug 15, 2024</t>
+  </si>
+  <si>
+    <t>Aug 22, 2024</t>
+  </si>
+  <si>
     <t>Aug 2, 2024</t>
   </si>
   <si>
-    <t>Jul 29, 2024</t>
-  </si>
-  <si>
-    <t>Aug 21, 2024</t>
-  </si>
-  <si>
-    <t>Aug 6, 2024</t>
-  </si>
-  <si>
-    <t>Aug 17, 2024</t>
-  </si>
-  <si>
-    <t>Aug 5, 2024</t>
-  </si>
-  <si>
-    <t>Aug 27, 2024</t>
-  </si>
-  <si>
-    <t>Jul 28, 2024</t>
-  </si>
-  <si>
-    <t>Aug 3, 2024</t>
-  </si>
-  <si>
-    <t>Jul 30, 2024</t>
-  </si>
-  <si>
-    <t>Aug 13, 2024</t>
-  </si>
-  <si>
-    <t>Aug 16, 2024</t>
-  </si>
-  <si>
-    <t>Aug 12, 2024</t>
-  </si>
-  <si>
-    <t>Aug 20, 2024</t>
-  </si>
-  <si>
-    <t>Aug 4, 2024</t>
-  </si>
-  <si>
-    <t>Aug 8, 2024</t>
-  </si>
-  <si>
-    <t>Aug 11, 2024</t>
-  </si>
-  <si>
-    <t>Aug 14, 2024</t>
-  </si>
-  <si>
-    <t>Aug 18, 2024</t>
-  </si>
-  <si>
-    <t>Aug 15, 2024</t>
-  </si>
-  <si>
-    <t>Aug 22, 2024</t>
-  </si>
-  <si>
     <t>Aug 26, 2024</t>
   </si>
   <si>
     <t>active</t>
+  </si>
+  <si>
+    <t>past_due</t>
   </si>
 </sst>
 </file>

</xml_diff>